<commit_message>
If, And, Or, Countif, countifs, sumif
</commit_message>
<xml_diff>
--- a/5. Logical/logical.xlsx
+++ b/5. Logical/logical.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\07_Videos\01_excel\Raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Advance_Excel_BI\5. Logical\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199F3840-01A7-4471-AF80-8219928A9B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="862"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="862" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AND OR" sheetId="2" r:id="rId1"/>
@@ -30,17 +31,28 @@
     <definedName name="UserChoice" localSheetId="3">#REF!</definedName>
     <definedName name="UserChoice">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="45">
   <si>
     <t>Example</t>
   </si>
@@ -178,12 +190,15 @@
   </si>
   <si>
     <t>&lt; 35 in any one subject</t>
+  </si>
+  <si>
+    <t>Student 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -323,7 +338,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -471,7 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -482,7 +497,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -512,66 +527,46 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -584,7 +579,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -611,7 +606,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -626,9 +621,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -641,7 +633,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -656,9 +648,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma 2" xfId="1"/>
+    <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -675,7 +673,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Welcome"/>
@@ -1513,36 +1511,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="3.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="0.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" style="17" customWidth="1"/>
-    <col min="11" max="11" width="3.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="13" max="15" width="11.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="1" max="2" width="3.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="0.6640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="3.6640625" style="17" customWidth="1"/>
+    <col min="11" max="11" width="3.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" customWidth="1"/>
+    <col min="13" max="15" width="11.6640625" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21" customWidth="1"/>
+    <col min="18" max="18" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="62"/>
+      <c r="C1" s="35"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -1550,331 +1550,331 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="62" t="s">
+      <c r="K1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
       <c r="AB1" s="15"/>
     </row>
-    <row r="2" spans="1:28" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:28" ht="33" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:28" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:28" ht="31.8" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="12"/>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="30" t="s">
+      <c r="Q3" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="R3" s="30" t="s">
+      <c r="R3" s="27" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14"/>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="46"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="38"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="O4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="26" t="s">
+      <c r="P4" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="Q4" s="26" t="s">
+      <c r="Q4" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="R4" s="26" t="s">
+      <c r="R4" s="23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="49"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="27">
+      <c r="M5" s="24">
         <v>99</v>
       </c>
-      <c r="N5" s="27">
+      <c r="N5" s="24">
         <v>83</v>
       </c>
-      <c r="O5" s="27">
+      <c r="O5" s="24">
         <v>85</v>
       </c>
-      <c r="P5" s="27" t="b">
+      <c r="P5" s="63" t="b">
         <f>M5=100</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="43" t="b">
+      <c r="Q5" s="64" t="b">
         <f>AND(M5&gt;75,N5&gt;75,O5&gt;75)</f>
         <v>1</v>
       </c>
-      <c r="R5" s="27" t="b">
+      <c r="R5" s="63" t="b">
         <f>OR(M5&lt;35,N5&lt;35,O5&lt;35)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="47"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="49"/>
-      <c r="L6" s="27" t="s">
+    <row r="6" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="39"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="41"/>
+      <c r="L6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="27">
+      <c r="M6" s="24">
         <v>65</v>
       </c>
-      <c r="N6" s="27">
+      <c r="N6" s="24">
         <v>53</v>
       </c>
-      <c r="O6" s="27">
+      <c r="O6" s="24">
         <v>43</v>
       </c>
-      <c r="P6" s="27" t="b">
+      <c r="P6" s="63" t="b">
         <f t="shared" ref="P6:P9" si="0">M6=100</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="27" t="b">
+      <c r="Q6" s="63" t="b">
         <f t="shared" ref="Q6:Q9" si="1">AND(M6&gt;75,N6&gt;75,O6&gt;75)</f>
         <v>0</v>
       </c>
-      <c r="R6" s="27" t="b">
+      <c r="R6" s="63" t="b">
         <f t="shared" ref="R6:R9" si="2">OR(M6&lt;35,N6&lt;35,O6&lt;35)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="47"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="49"/>
-      <c r="L7" s="27" t="s">
+    <row r="7" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="39"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="41"/>
+      <c r="L7" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="27">
+      <c r="M7" s="24">
         <v>85</v>
       </c>
-      <c r="N7" s="27">
+      <c r="N7" s="24">
         <v>80</v>
       </c>
-      <c r="O7" s="27">
+      <c r="O7" s="24">
         <v>79</v>
       </c>
-      <c r="P7" s="27" t="b">
+      <c r="P7" s="63" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q7" s="43" t="b">
+      <c r="Q7" s="64" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R7" s="27" t="b">
+      <c r="R7" s="63" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="47"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="49"/>
-      <c r="L8" s="27" t="s">
+    <row r="8" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="39"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="41"/>
+      <c r="L8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="27">
+      <c r="M8" s="24">
         <v>100</v>
       </c>
-      <c r="N8" s="27">
+      <c r="N8" s="24">
         <v>99</v>
       </c>
-      <c r="O8" s="27">
+      <c r="O8" s="24">
         <v>82</v>
       </c>
-      <c r="P8" s="43" t="b">
+      <c r="P8" s="64" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q8" s="43" t="b">
+      <c r="Q8" s="64" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R8" s="27" t="b">
+      <c r="R8" s="63" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="47"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="49"/>
-      <c r="L9" s="27" t="s">
+    <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="39"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="41"/>
+      <c r="L9" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="27">
+      <c r="M9" s="24">
         <v>45</v>
       </c>
-      <c r="N9" s="27">
+      <c r="N9" s="24">
         <v>60</v>
       </c>
-      <c r="O9" s="27">
+      <c r="O9" s="24">
         <v>30</v>
       </c>
-      <c r="P9" s="27" t="b">
+      <c r="P9" s="63" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q9" s="27" t="b">
+      <c r="Q9" s="63" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R9" s="43" t="b">
+      <c r="R9" s="64" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="47"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="49"/>
-    </row>
-    <row r="11" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="41"/>
+    </row>
+    <row r="11" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="52"/>
-    </row>
-    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="42"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="44"/>
+    </row>
+    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B12" s="4"/>
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C13" s="13"/>
     </row>
-    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="55"/>
-    </row>
-    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
+    </row>
+    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="58"/>
-    </row>
-    <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="50"/>
+    </row>
+    <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="58"/>
-    </row>
-    <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="56"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="58"/>
-    </row>
-    <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="56"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="58"/>
-    </row>
-    <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="56"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="58"/>
-    </row>
-    <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="56"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="58"/>
-    </row>
-    <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="59"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="61"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
+    </row>
+    <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="50"/>
+    </row>
+    <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
+    </row>
+    <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50"/>
+    </row>
+    <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
+    </row>
+    <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="C4:G11"/>
     <mergeCell ref="C14:G21"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1882,31 +1882,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="3.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="0.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" style="17" customWidth="1"/>
-    <col min="11" max="11" width="3.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="13" max="15" width="11.7109375" customWidth="1"/>
-    <col min="16" max="16" width="21.85546875" customWidth="1"/>
-    <col min="17" max="17" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="1" max="2" width="3.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="0.6640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="3.6640625" style="17" customWidth="1"/>
+    <col min="11" max="11" width="3.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" customWidth="1"/>
+    <col min="13" max="15" width="11.6640625" customWidth="1"/>
+    <col min="16" max="16" width="21.88671875" customWidth="1"/>
+    <col min="17" max="17" width="27.77734375" customWidth="1"/>
+    <col min="18" max="18" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>14</v>
@@ -1919,424 +1921,412 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="62" t="s">
+      <c r="K1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="62"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
       <c r="Z1" s="15"/>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:26" ht="48" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:26" ht="15" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:26" ht="70.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="12"/>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" s="30" t="s">
+      <c r="Q3" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="30" t="s">
+      <c r="R3" s="27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14"/>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="65"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="O4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="26" t="s">
+      <c r="P4" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="26" t="s">
+      <c r="Q4" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="26" t="s">
+      <c r="R4" s="23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="68"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="59"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="27">
+      <c r="M5" s="24">
         <v>99</v>
       </c>
-      <c r="N5" s="27">
+      <c r="N5" s="24">
         <v>83</v>
       </c>
-      <c r="O5" s="27">
+      <c r="O5" s="24">
         <v>85</v>
       </c>
-      <c r="P5" s="24" t="str">
+      <c r="P5" s="22" t="str">
         <f>IF(M5&gt;=75,"A","B")</f>
         <v>A</v>
       </c>
-      <c r="Q5" s="24" t="str">
-        <f>IF(N5&gt;=85,"A",IF(N5&lt;60,"C","B"))</f>
+      <c r="Q5" s="22" t="str">
+        <f>IF(N5&gt;=85,"A",IF(N5&gt;=60,"B","C"))</f>
         <v>B</v>
       </c>
-      <c r="R5" s="24"/>
-    </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="66"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="68"/>
-      <c r="L6" s="27" t="s">
+      <c r="R5" s="22"/>
+    </row>
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="57"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="59"/>
+      <c r="L6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="27">
+      <c r="M6" s="24">
         <v>65</v>
       </c>
-      <c r="N6" s="27">
+      <c r="N6" s="24">
         <v>53</v>
       </c>
-      <c r="O6" s="27">
+      <c r="O6" s="24">
         <v>43</v>
       </c>
-      <c r="P6" s="24" t="str">
+      <c r="P6" s="22" t="str">
         <f t="shared" ref="P6:P9" si="0">IF(M6&gt;=75,"A","B")</f>
         <v>B</v>
       </c>
-      <c r="Q6" s="24" t="str">
-        <f t="shared" ref="Q6:Q9" si="1">IF(N6&gt;=85,"A",IF(N6&lt;60,"C","B"))</f>
+      <c r="Q6" s="22" t="str">
+        <f>IF(N6&gt;=85,"A",IF(N6&lt;60,"C","B"))</f>
         <v>C</v>
       </c>
-      <c r="R6" s="24"/>
-    </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="66"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="68"/>
-      <c r="L7" s="27" t="s">
+      <c r="R6" s="22"/>
+    </row>
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="57"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="59"/>
+      <c r="L7" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="27">
+      <c r="M7" s="24">
         <v>85</v>
       </c>
-      <c r="N7" s="27">
+      <c r="N7" s="24">
         <v>80</v>
       </c>
-      <c r="O7" s="27">
+      <c r="O7" s="24">
         <v>79</v>
       </c>
-      <c r="P7" s="24" t="str">
+      <c r="P7" s="22" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
       </c>
-      <c r="Q7" s="24" t="str">
+      <c r="Q7" s="22" t="str">
+        <f t="shared" ref="Q7:Q9" si="1">IF(N7&gt;=85,"A",IF(N7&lt;60,"C","B"))</f>
+        <v>B</v>
+      </c>
+      <c r="R7" s="22"/>
+    </row>
+    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="57"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="59"/>
+      <c r="L8" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="24">
+        <v>100</v>
+      </c>
+      <c r="N8" s="24">
+        <v>99</v>
+      </c>
+      <c r="O8" s="24">
+        <v>82</v>
+      </c>
+      <c r="P8" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+      <c r="Q8" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
+      </c>
+      <c r="R8" s="22"/>
+    </row>
+    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="57"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="59"/>
+      <c r="L9" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="24">
+        <v>45</v>
+      </c>
+      <c r="N9" s="24">
+        <v>60</v>
+      </c>
+      <c r="O9" s="24">
+        <v>30</v>
+      </c>
+      <c r="P9" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
+      <c r="Q9" s="22" t="str">
         <f t="shared" si="1"/>
         <v>B</v>
       </c>
-      <c r="R7" s="24"/>
-    </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="66"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="68"/>
-      <c r="L8" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="27">
-        <v>100</v>
-      </c>
-      <c r="N8" s="27">
-        <v>99</v>
-      </c>
-      <c r="O8" s="27">
-        <v>82</v>
-      </c>
-      <c r="P8" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>A</v>
-      </c>
-      <c r="Q8" s="24" t="str">
-        <f t="shared" si="1"/>
-        <v>A</v>
-      </c>
-      <c r="R8" s="24"/>
-    </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="66"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="68"/>
-      <c r="L9" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="27">
-        <v>45</v>
-      </c>
-      <c r="N9" s="27">
-        <v>60</v>
-      </c>
-      <c r="O9" s="27">
-        <v>30</v>
-      </c>
-      <c r="P9" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>B</v>
-      </c>
-      <c r="Q9" s="24" t="str">
-        <f t="shared" si="1"/>
-        <v>B</v>
-      </c>
-      <c r="R9" s="24"/>
-    </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="66"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="68"/>
-    </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R9" s="22"/>
+    </row>
+    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="57"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
+    </row>
+    <row r="11" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="71"/>
-    </row>
-    <row r="12" spans="1:26" ht="38.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="62"/>
+    </row>
+    <row r="12" spans="1:26" ht="38.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B12" s="4"/>
       <c r="C12" s="12"/>
-      <c r="P12" s="30" t="s">
+      <c r="P12" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="Q12" s="42" t="s">
+      <c r="Q12" s="34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C13" s="13"/>
-      <c r="L13" s="31" t="s">
+      <c r="L13" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="M13" s="31" t="s">
+      <c r="M13" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="N13" s="31" t="s">
+      <c r="N13" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="O13" s="32" t="s">
+      <c r="O13" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="P13" s="32" t="s">
+      <c r="P13" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="Q13" s="32" t="s">
+      <c r="Q13" s="28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="55"/>
-      <c r="L14" s="33" t="s">
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
+      <c r="L14" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M14" s="33">
+      <c r="M14" s="29">
         <v>99</v>
       </c>
-      <c r="N14" s="33">
+      <c r="N14" s="29">
         <v>83</v>
       </c>
-      <c r="O14" s="33">
+      <c r="O14" s="29">
         <v>85</v>
       </c>
-      <c r="P14" s="33" t="str">
-        <f>IF(AND(O14&gt;75,N14&gt;75,M14&gt;75),"Passed with Distinction","")</f>
-        <v>Passed with Distinction</v>
-      </c>
-      <c r="Q14" s="33" t="str">
+      <c r="P14" s="29" t="str">
+        <f>IF(AND(M14&gt;75,N14&gt;75,O14&gt;75),"Passed with distinction"," ")</f>
+        <v>Passed with distinction</v>
+      </c>
+      <c r="Q14" s="29" t="str">
         <f>IF(OR(O14&lt;35,N14&lt;35,M14&lt;35),"Failed","Promoted to next class")</f>
         <v>Promoted to next class</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="58"/>
-      <c r="L15" s="33" t="s">
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="50"/>
+      <c r="L15" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="M15" s="33">
+      <c r="M15" s="29">
         <v>65</v>
       </c>
-      <c r="N15" s="33">
+      <c r="N15" s="29">
         <v>53</v>
       </c>
-      <c r="O15" s="33">
+      <c r="O15" s="29">
         <v>43</v>
       </c>
-      <c r="P15" s="33" t="str">
-        <f t="shared" ref="P15:P18" si="2">IF(AND(O15&gt;75,N15&gt;75,M15&gt;75),"Passed with Distinction","")</f>
-        <v/>
-      </c>
-      <c r="Q15" s="33" t="str">
-        <f t="shared" ref="Q15:Q18" si="3">IF(OR(O15&lt;35,N15&lt;35,M15&lt;35),"Failed","Promoted to next class")</f>
-        <v>Promoted to next class</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P15" s="29" t="str">
+        <f t="shared" ref="P15:P18" si="2">IF(AND(M15&gt;75,N15&gt;75,O15&gt;75),"Passed with distinction"," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Q15" s="29"/>
+    </row>
+    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="58"/>
-      <c r="L16" s="33" t="s">
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
+      <c r="L16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="M16" s="33">
+      <c r="M16" s="29">
         <v>85</v>
       </c>
-      <c r="N16" s="33">
+      <c r="N16" s="29">
         <v>80</v>
       </c>
-      <c r="O16" s="33">
+      <c r="O16" s="29">
         <v>79</v>
       </c>
-      <c r="P16" s="33" t="str">
+      <c r="P16" s="29" t="str">
         <f t="shared" si="2"/>
-        <v>Passed with Distinction</v>
-      </c>
-      <c r="Q16" s="33" t="str">
-        <f t="shared" si="3"/>
-        <v>Promoted to next class</v>
-      </c>
-    </row>
-    <row r="17" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="56"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="58"/>
-      <c r="L17" s="33" t="s">
+        <v>Passed with distinction</v>
+      </c>
+      <c r="Q16" s="29"/>
+    </row>
+    <row r="17" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="50"/>
+      <c r="L17" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="M17" s="33">
+      <c r="M17" s="29">
         <v>100</v>
       </c>
-      <c r="N17" s="33">
+      <c r="N17" s="29">
         <v>99</v>
       </c>
-      <c r="O17" s="33">
+      <c r="O17" s="29">
         <v>82</v>
       </c>
-      <c r="P17" s="33" t="str">
+      <c r="P17" s="29" t="str">
         <f t="shared" si="2"/>
-        <v>Passed with Distinction</v>
-      </c>
-      <c r="Q17" s="33" t="str">
-        <f t="shared" si="3"/>
-        <v>Promoted to next class</v>
-      </c>
-    </row>
-    <row r="18" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="56"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="58"/>
-      <c r="L18" s="33" t="s">
+        <v>Passed with distinction</v>
+      </c>
+      <c r="Q17" s="29"/>
+    </row>
+    <row r="18" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
+      <c r="L18" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="M18" s="33">
+      <c r="M18" s="29">
         <v>45</v>
       </c>
-      <c r="N18" s="33">
+      <c r="N18" s="29">
         <v>60</v>
       </c>
-      <c r="O18" s="33">
+      <c r="O18" s="29">
         <v>30</v>
       </c>
-      <c r="P18" s="33" t="str">
+      <c r="P18" s="29" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="Q18" s="33" t="str">
-        <f t="shared" si="3"/>
-        <v>Failed</v>
-      </c>
-    </row>
-    <row r="19" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="56"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="58"/>
-    </row>
-    <row r="20" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="56"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="58"/>
-    </row>
-    <row r="21" spans="3:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="59"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="61"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="Q18" s="29"/>
+    </row>
+    <row r="19" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50"/>
+    </row>
+    <row r="20" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
+    </row>
+    <row r="21" spans="3:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2356,31 +2346,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="3.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="0.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" style="17" customWidth="1"/>
-    <col min="11" max="11" width="3.7109375" customWidth="1"/>
+    <col min="1" max="2" width="3.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="0.6640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="3.6640625" style="17" customWidth="1"/>
+    <col min="11" max="11" width="3.6640625" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="15" width="11.7109375" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="11.6640625" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>15</v>
@@ -2393,382 +2385,401 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="62" t="s">
+      <c r="K1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
       <c r="AA1" s="15"/>
     </row>
-    <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:27" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="12"/>
     </row>
-    <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14"/>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="65"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="O4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="26" t="s">
+      <c r="P4" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="26" t="s">
+      <c r="Q4" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="26" t="s">
+      <c r="R4" s="23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="68"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="59"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="27">
+      <c r="M5" s="24">
         <v>99</v>
       </c>
-      <c r="N5" s="27">
+      <c r="N5" s="24">
         <v>83</v>
       </c>
-      <c r="O5" s="27">
+      <c r="O5" s="24">
         <v>85</v>
       </c>
-      <c r="P5" s="24" t="str">
+      <c r="P5" s="22" t="str">
         <f>IF(M5&gt;=75,"A","B")</f>
         <v>A</v>
       </c>
-      <c r="Q5" s="24" t="str">
+      <c r="Q5" s="22" t="str">
         <f>IF(N5&gt;=85,"A",(IF(N5&lt;60,"C","B")))</f>
         <v>B</v>
       </c>
-      <c r="R5" s="24" t="str">
+      <c r="R5" s="22" t="str">
         <f>IF(O5&gt;=85,"A",IF(AND(O5&lt;85,O5&gt;=60),"B","C"))</f>
         <v>A</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="66"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="68"/>
-      <c r="L6" s="27" t="s">
+    <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="57"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="59"/>
+      <c r="L6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="27">
+      <c r="M6" s="24">
         <v>65</v>
       </c>
-      <c r="N6" s="27">
+      <c r="N6" s="24">
         <v>53</v>
       </c>
-      <c r="O6" s="27">
+      <c r="O6" s="24">
         <v>43</v>
       </c>
-      <c r="P6" s="24" t="str">
+      <c r="P6" s="22" t="str">
         <f t="shared" ref="P6:P9" si="0">IF(M6&gt;=75,"A","B")</f>
         <v>B</v>
       </c>
-      <c r="Q6" s="24" t="str">
+      <c r="Q6" s="22" t="str">
         <f t="shared" ref="Q6:Q9" si="1">IF(N6&gt;=85,"A",(IF(N6&lt;60,"C","B")))</f>
         <v>C</v>
       </c>
-      <c r="R6" s="24" t="str">
+      <c r="R6" s="22" t="str">
         <f t="shared" ref="R6:R9" si="2">IF(O6&gt;=85,"A",IF(AND(O6&lt;85,O6&gt;=60),"B","C"))</f>
         <v>C</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="66"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="68"/>
-      <c r="L7" s="27" t="s">
+    <row r="7" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="57"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="59"/>
+      <c r="L7" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="27">
+      <c r="M7" s="24">
         <v>85</v>
       </c>
-      <c r="N7" s="27">
+      <c r="N7" s="24">
         <v>80</v>
       </c>
-      <c r="O7" s="27">
+      <c r="O7" s="24">
         <v>79</v>
       </c>
-      <c r="P7" s="24" t="str">
+      <c r="P7" s="22" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
       </c>
-      <c r="Q7" s="24" t="str">
+      <c r="Q7" s="22" t="str">
         <f t="shared" si="1"/>
         <v>B</v>
       </c>
-      <c r="R7" s="24" t="str">
+      <c r="R7" s="22" t="str">
         <f t="shared" si="2"/>
         <v>B</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="66"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="68"/>
-      <c r="L8" s="27" t="s">
+    <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="57"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="59"/>
+      <c r="L8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="27">
+      <c r="M8" s="24">
         <v>100</v>
       </c>
-      <c r="N8" s="27">
+      <c r="N8" s="24">
         <v>99</v>
       </c>
-      <c r="O8" s="27">
+      <c r="O8" s="24">
         <v>82</v>
       </c>
-      <c r="P8" s="24" t="str">
+      <c r="P8" s="22" t="str">
         <f t="shared" si="0"/>
         <v>A</v>
       </c>
-      <c r="Q8" s="24" t="str">
+      <c r="Q8" s="22" t="str">
         <f t="shared" si="1"/>
         <v>A</v>
       </c>
-      <c r="R8" s="24" t="str">
+      <c r="R8" s="22" t="str">
         <f t="shared" si="2"/>
         <v>B</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="66"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="68"/>
-      <c r="L9" s="27" t="s">
+    <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="57"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="59"/>
+      <c r="L9" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="27">
+      <c r="M9" s="24">
         <v>45</v>
       </c>
-      <c r="N9" s="27">
+      <c r="N9" s="24">
         <v>60</v>
       </c>
-      <c r="O9" s="27">
+      <c r="O9" s="24">
         <v>30</v>
       </c>
-      <c r="P9" s="24" t="str">
+      <c r="P9" s="22" t="str">
         <f t="shared" si="0"/>
         <v>B</v>
       </c>
-      <c r="Q9" s="24" t="str">
+      <c r="Q9" s="22" t="str">
         <f t="shared" si="1"/>
         <v>B</v>
       </c>
-      <c r="R9" s="24" t="str">
+      <c r="R9" s="22" t="str">
         <f t="shared" si="2"/>
         <v>C</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="66"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="68"/>
-    </row>
-    <row r="11" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="57"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
+      <c r="L10" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" s="24">
+        <v>95</v>
+      </c>
+      <c r="N10" s="24">
+        <v>95</v>
+      </c>
+      <c r="O10" s="24">
+        <v>99</v>
+      </c>
+      <c r="P10" s="22" t="str">
+        <f t="shared" ref="P10" si="3">IF(M10&gt;=75,"A","B")</f>
+        <v>A</v>
+      </c>
+      <c r="Q10" s="22" t="str">
+        <f t="shared" ref="Q10" si="4">IF(N10&gt;=85,"A",(IF(N10&lt;60,"C","B")))</f>
+        <v>A</v>
+      </c>
+      <c r="R10" s="22" t="str">
+        <f t="shared" ref="R10" si="5">IF(O10&gt;=85,"A",IF(AND(O10&lt;85,O10&gt;=60),"B","C"))</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="71"/>
-    </row>
-    <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="62"/>
+    </row>
+    <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B12" s="4"/>
       <c r="C12" s="12"/>
-      <c r="L12" s="29" t="s">
+      <c r="L12" s="26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C13" s="13"/>
     </row>
-    <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="55"/>
-      <c r="L14" s="31" t="s">
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
+      <c r="L14" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="M14" s="31" t="s">
+      <c r="M14" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="N14" s="31" t="s">
+      <c r="N14" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="O14" s="32" t="s">
+      <c r="O14" s="28" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="58"/>
-      <c r="L15" s="24" t="s">
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="50"/>
+      <c r="L15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="M15" s="27">
-        <f>COUNTIF(P$5:P$9,$L15)</f>
+      <c r="M15" s="24">
+        <f>COUNTIF($P$5:$P$9,L15)</f>
         <v>3</v>
       </c>
-      <c r="N15" s="27">
-        <f t="shared" ref="N15:O15" si="3">COUNTIF(Q$5:Q$9,$L15)</f>
+      <c r="N15" s="24">
+        <f>COUNTIF($Q$5:$Q$9,L15)</f>
         <v>1</v>
       </c>
-      <c r="O15" s="27">
-        <f t="shared" si="3"/>
+      <c r="O15" s="24"/>
+    </row>
+    <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="6"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
+      <c r="L16" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" s="24">
+        <f t="shared" ref="M16:M17" si="6">COUNTIF($P$5:$P$9,L16)</f>
+        <v>2</v>
+      </c>
+      <c r="N16" s="24">
+        <f t="shared" ref="N16:N17" si="7">COUNTIF($Q$5:$Q$9,L16)</f>
+        <v>3</v>
+      </c>
+      <c r="O16" s="24"/>
+    </row>
+    <row r="17" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="50"/>
+      <c r="L17" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="M17" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="24">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="58"/>
-      <c r="L16" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="M16" s="27">
-        <f t="shared" ref="M16:M17" si="4">COUNTIF($P$5:$P$9,L16)</f>
-        <v>2</v>
-      </c>
-      <c r="N16" s="27">
-        <f t="shared" ref="N16:N17" si="5">COUNTIF(Q$5:Q$9,$L16)</f>
-        <v>3</v>
-      </c>
-      <c r="O16" s="27">
-        <f t="shared" ref="O16:O17" si="6">COUNTIF(R$5:R$9,$L16)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="56"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="58"/>
-      <c r="L17" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="M17" s="27">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="27">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="O17" s="27">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="56"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="58"/>
-    </row>
-    <row r="19" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="56"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="58"/>
-      <c r="L19" s="29" t="s">
+      <c r="O17" s="24"/>
+    </row>
+    <row r="18" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
+    </row>
+    <row r="19" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50"/>
+      <c r="L19" s="26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="56"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="58"/>
-      <c r="L20" s="34"/>
-    </row>
-    <row r="21" spans="3:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="59"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="61"/>
-      <c r="L21" s="35" t="s">
+    <row r="20" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
+      <c r="L20" s="30"/>
+    </row>
+    <row r="21" spans="3:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="53"/>
+      <c r="L21" s="31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L22" s="36" t="s">
+    <row r="22" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L22" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="M22" s="21">
+      <c r="M22" s="20">
         <f>COUNTIFS(M5:M9,L22,N5:N9,L22,O5:O9,L22)</f>
         <v>0</v>
+      </c>
+      <c r="N22">
+        <f>COUNTIFS(M5:M10,L22,N5:N10,L22,O5:O10,L22)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2790,28 +2801,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="3.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="0.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" style="17" customWidth="1"/>
-    <col min="11" max="11" width="3.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="18" width="11.7109375" customWidth="1"/>
+    <col min="1" max="2" width="3.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="0.6640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="3.6640625" style="17" customWidth="1"/>
+    <col min="11" max="11" width="3.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+    <col min="13" max="18" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -2824,337 +2837,337 @@
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="62" t="s">
+      <c r="K1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="62"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
       <c r="Z1" s="15"/>
     </row>
-    <row r="2" spans="1:26" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:26" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="12"/>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14"/>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="65"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="14"/>
       <c r="I4" s="10"/>
       <c r="J4" s="18"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="39" t="s">
+      <c r="L4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="39" t="s">
+      <c r="M4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="39" t="s">
+      <c r="N4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="40" t="s">
+      <c r="O4" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="40" t="s">
+      <c r="P4" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="Q4" s="40" t="s">
+      <c r="Q4" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="R4" s="40" t="s">
+      <c r="R4" s="33" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="68"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="59"/>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="19"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="41" t="s">
+      <c r="L5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="41">
+      <c r="M5" s="20">
         <v>99</v>
       </c>
-      <c r="N5" s="41">
+      <c r="N5" s="20">
         <v>83</v>
       </c>
-      <c r="O5" s="41">
+      <c r="O5" s="20">
         <v>85</v>
       </c>
-      <c r="P5" s="41" t="b">
+      <c r="P5" s="20" t="b">
         <f>M5=100</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="41" t="b">
+      <c r="Q5" s="20" t="b">
         <f>AND(M5&gt;75,N5&gt;75,O5&gt;75)</f>
         <v>1</v>
       </c>
-      <c r="R5" s="41" t="b">
+      <c r="R5" s="20" t="b">
         <f>OR(M5&lt;35,N5&lt;35,O5&lt;35)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="66"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="68"/>
-      <c r="L6" s="41" t="s">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="57"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="59"/>
+      <c r="L6" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="41">
+      <c r="M6" s="20">
         <v>65</v>
       </c>
-      <c r="N6" s="41">
+      <c r="N6" s="20">
         <v>53</v>
       </c>
-      <c r="O6" s="41">
+      <c r="O6" s="20">
         <v>43</v>
       </c>
-      <c r="P6" s="41" t="b">
+      <c r="P6" s="20" t="b">
         <f t="shared" ref="P6:P9" si="0">M6=100</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="41" t="b">
+      <c r="Q6" s="20" t="b">
         <f t="shared" ref="Q6:Q9" si="1">AND(M6&gt;75,N6&gt;75,O6&gt;75)</f>
         <v>0</v>
       </c>
-      <c r="R6" s="41" t="b">
+      <c r="R6" s="20" t="b">
         <f t="shared" ref="R6:R9" si="2">OR(M6&lt;35,N6&lt;35,O6&lt;35)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="66"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="68"/>
-      <c r="L7" s="41" t="s">
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="57"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="59"/>
+      <c r="L7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="41">
+      <c r="M7" s="20">
         <v>85</v>
       </c>
-      <c r="N7" s="41">
+      <c r="N7" s="20">
         <v>80</v>
       </c>
-      <c r="O7" s="41">
+      <c r="O7" s="20">
         <v>79</v>
       </c>
-      <c r="P7" s="41" t="b">
+      <c r="P7" s="20" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q7" s="41" t="b">
+      <c r="Q7" s="20" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R7" s="41" t="b">
+      <c r="R7" s="20" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="66"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="68"/>
-      <c r="L8" s="41" t="s">
+    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="57"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="59"/>
+      <c r="L8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="41">
+      <c r="M8" s="20">
         <v>100</v>
       </c>
-      <c r="N8" s="41">
+      <c r="N8" s="20">
         <v>99</v>
       </c>
-      <c r="O8" s="41">
+      <c r="O8" s="20">
         <v>82</v>
       </c>
-      <c r="P8" s="41" t="b">
+      <c r="P8" s="20" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q8" s="41" t="b">
+      <c r="Q8" s="20" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R8" s="41" t="b">
+      <c r="R8" s="20" t="b">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="66"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="68"/>
-      <c r="L9" s="41" t="s">
+    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="57"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="59"/>
+      <c r="L9" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="41">
+      <c r="M9" s="20">
         <v>45</v>
       </c>
-      <c r="N9" s="41">
+      <c r="N9" s="20">
         <v>60</v>
       </c>
-      <c r="O9" s="41">
+      <c r="O9" s="66">
         <v>30</v>
       </c>
-      <c r="P9" s="41" t="b">
+      <c r="P9" s="20" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q9" s="41" t="b">
+      <c r="Q9" s="20" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R9" s="41" t="b">
+      <c r="R9" s="20" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="66"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="68"/>
-    </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="57"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
+    </row>
+    <row r="11" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="5"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="71"/>
-      <c r="L11" s="29" t="s">
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="62"/>
+      <c r="L11" s="26" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B12" s="4"/>
       <c r="C12" s="12"/>
-      <c r="L12" s="28"/>
-    </row>
-    <row r="13" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L12" s="25"/>
+    </row>
+    <row r="13" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C13" s="13"/>
-      <c r="L13" s="37" t="s">
+      <c r="L13" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="37" t="s">
+      <c r="M13" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="N13" s="38" t="s">
+      <c r="N13" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="O13" s="37" t="s">
+      <c r="O13" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="55"/>
-      <c r="L14" s="37" t="b">
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
+      <c r="L14" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="M14" s="23">
-        <f>SUMIF($R$5:R$9,$L$14,M5:M9)</f>
+      <c r="M14" s="21">
+        <f>SUMIF($R$5:$R$9,$L$14,M5:M9)</f>
         <v>349</v>
       </c>
-      <c r="N14" s="23">
-        <f ca="1">SUMIF($R$5:S$9,$L$14,N5:N9)</f>
+      <c r="N14" s="21">
+        <f t="shared" ref="N14:O14" si="3">SUMIF($R$5:$R$9,$L$14,N5:N9)</f>
         <v>315</v>
       </c>
-      <c r="O14" s="23">
-        <f ca="1">SUMIF($R$5:T$9,$L$14,O5:O9)</f>
+      <c r="O14" s="21">
+        <f t="shared" si="3"/>
         <v>289</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="58"/>
-    </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="48"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="50"/>
+    </row>
+    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="58"/>
-    </row>
-    <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="56"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="58"/>
-    </row>
-    <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="56"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="58"/>
-    </row>
-    <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="56"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="58"/>
-    </row>
-    <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="56"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="58"/>
-    </row>
-    <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="59"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="61"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
+    </row>
+    <row r="17" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="48"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="50"/>
+    </row>
+    <row r="18" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
+    </row>
+    <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50"/>
+    </row>
+    <row r="20" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="50"/>
+    </row>
+    <row r="21" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>